<commit_message>
A1 - A6 evidences
</commit_message>
<xml_diff>
--- a/EmreNOP/evidence.xlsx
+++ b/EmreNOP/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="50">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -100,34 +100,85 @@
     <t xml:space="preserve">ClassID</t>
   </si>
   <si>
-    <t xml:space="preserve">tx hash on irisnet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">class id you issued</t>
+    <t xml:space="preserve">6B577B760234031F076DE19D568C4CF6474C1D707F9D3AB0042EA7A94AF3B5F0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emrenop1</t>
   </si>
   <si>
     <t xml:space="preserve">NFTID</t>
   </si>
   <si>
-    <t xml:space="preserve">nft id you minted</t>
+    <t xml:space="preserve">441E44BCB9B294C3DF16D5DB31B2040D6E8CB50CA96AC1E8ED28E00E3161047D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emrenopnft1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">140031CF079F8549A0C39F1FE7633DE2B1FC25BB234D0B9944329C3A4008672A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emrenopnft2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90D1267BC118311DF4FBA60C48C4DC63586AA6ADE835B1DA3C96465A51BE222B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emrenopnft3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4EDBEB466803A07ED20BBD497194206ADF6DFD3785E97BE473F8CC5F74C4D4B9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emrenopnft4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DB910A7380711547052748E4295D82A8C20B38D8C7C9C3B622450BBE18A52983</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emrenopnft5</t>
   </si>
   <si>
     <t xml:space="preserve">ChainID</t>
   </si>
   <si>
-    <t xml:space="preserve">ibc class on dest chain</t>
+    <t xml:space="preserve">BB73FAA5DD768AA7BA35C44ED97A783C44DD7B3C701CA410F55F0811AC23E220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-89/emrenop1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uni-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06167B0C37824B3C712ECCBBD4EED5F99C8884E510239FBC79CCF16D4CE91A83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F0F70701233303EF29D6E1B1F9AB2D6948D3831A61AC4E446130657B930A6B31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C800F3B8F8683EE8EE1DCE16A8BB9607310C18E72FBFA20CAF8FA0A64CAF94C3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gon-flixnet-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38CDF824F30D3CED2C290440CB6DC3A31486A46DCD1EC74A653750F142EE5D45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uni-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A98B6229BE10C8630B091B11F0832CC6A711714DB4630BF3B31015EA8B1C477A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/7937EB04B868B10EC4674C63CCF8183BC56B6E723E8B0F5C54FDF2AE8AC72A04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc class on chain</t>
   </si>
   <si>
     <t xml:space="preserve">nft id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dest chain id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tx hash on dest chain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ibc class on chain</t>
   </si>
   <si>
     <t xml:space="preserve">tx hash on that chain</t>
@@ -152,7 +203,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -181,6 +232,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -252,7 +309,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -275,6 +332,14 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -356,14 +421,14 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="18.15"/>
@@ -462,10 +527,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -506,10 +571,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -550,10 +615,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -594,10 +659,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -633,25 +698,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -687,25 +752,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -741,25 +806,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -795,25 +860,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -849,25 +914,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -903,25 +968,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -943,7 +1008,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -963,7 +1028,7 @@
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1000,25 +1065,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1054,25 +1119,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1109,12 +1174,12 @@
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1151,12 +1216,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1193,12 +1258,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1235,12 +1300,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1259,10 +1324,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1283,14 +1348,58 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>21</v>
+      <c r="C2" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1309,10 +1418,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1333,22 +1442,53 @@
         <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="D3" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1366,10 +1506,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1390,23 +1530,24 @@
         <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>18</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
+        <v>28</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1426,7 +1567,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1447,21 +1588,21 @@
         <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>25</v>
+      <c r="D2" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1482,8 +1623,8 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1505,21 +1646,21 @@
         <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>25</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1560,10 +1701,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1604,10 +1745,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stage1 format error fix and Stage2 evidences
</commit_message>
<xml_diff>
--- a/EmreNOP/evidence.xlsx
+++ b/EmreNOP/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="51">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -109,76 +109,79 @@
     <t xml:space="preserve">NFTID</t>
   </si>
   <si>
-    <t xml:space="preserve">441E44BCB9B294C3DF16D5DB31B2040D6E8CB50CA96AC1E8ED28E00E3161047D</t>
+    <t xml:space="preserve">4EDBEB466803A07ED20BBD497194206ADF6DFD3785E97BE473F8CC5F74C4D4B9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emrenopnft4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChainID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F0F70701233303EF29D6E1B1F9AB2D6948D3831A61AC4E446130657B930A6B31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">juno1zk6ryvvc0ymj5dmedg38qsayhg93mwaxg2xh77frnc8fda6m4wsqjj628d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uni-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C800F3B8F8683EE8EE1DCE16A8BB9607310C18E72FBFA20CAF8FA0A64CAF94C3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/7937EB04B868B10EC4674C63CCF8183BC56B6E723E8B0F5C54FDF2AE8AC72A04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gon-flixnet-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38CDF824F30D3CED2C290440CB6DC3A31486A46DCD1EC74A653750F142EE5D45</t>
   </si>
   <si>
     <t xml:space="preserve">emrenopnft1</t>
   </si>
   <si>
-    <t xml:space="preserve">140031CF079F8549A0C39F1FE7633DE2B1FC25BB234D0B9944329C3A4008672A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emrenopnft2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">90D1267BC118311DF4FBA60C48C4DC63586AA6ADE835B1DA3C96465A51BE222B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emrenopnft3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4EDBEB466803A07ED20BBD497194206ADF6DFD3785E97BE473F8CC5F74C4D4B9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emrenopnft4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DB910A7380711547052748E4295D82A8C20B38D8C7C9C3B622450BBE18A52983</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emrenopnft5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChainID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BB73FAA5DD768AA7BA35C44ED97A783C44DD7B3C701CA410F55F0811AC23E220</t>
-  </si>
-  <si>
-    <t xml:space="preserve">juno1zk6ryvvc0ymj5dmedg38qsayhg93mwaxg2xh77frnc8fda6m4wsqjj628d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uni-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06167B0C37824B3C712ECCBBD4EED5F99C8884E510239FBC79CCF16D4CE91A83</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F0F70701233303EF29D6E1B1F9AB2D6948D3831A61AC4E446130657B930A6B31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C800F3B8F8683EE8EE1DCE16A8BB9607310C18E72FBFA20CAF8FA0A64CAF94C3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ibc/7937EB04B868B10EC4674C63CCF8183BC56B6E723E8B0F5C54FDF2AE8AC72A04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gon-flixnet-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">38CDF824F30D3CED2C290440CB6DC3A31486A46DCD1EC74A653750F142EE5D45</t>
-  </si>
-  <si>
     <t xml:space="preserve">uni-6</t>
   </si>
   <si>
     <t xml:space="preserve">A98B6229BE10C8630B091B11F0832CC6A711714DB4630BF3B31015EA8B1C477A</t>
   </si>
   <si>
-    <t xml:space="preserve">ibc class on chain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nft id</t>
+    <t xml:space="preserve">ibc/5671C790FBC80D22BDDA8F2F6908B18F75BD74F157BA61706080EA805C2EB4D3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emrenopnftagoric1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/D553FA0825E13CFDFB5F0CDAA7ED668E99E9A5D960DE1960F77A08D387792CBF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emrenopnftagoric2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/357E12AA988AD4420CF3F97FA1788C45CBE6C270C8F8EAD4CDB6A0061D6FCBE9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emrenopnftmina1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/A2498473B78C34030CF1C3D61CCDCDB8784A88DEE429F5426BABE101F7D144FF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emrenopnftzksnark1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/8F92273E547AA3CBE322579F2BF44BD3A344F6FECCF346A07E94F24B95CA4982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emrenopnftavax1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/C4BEA9AF1E84EDDB4014ABC5E7B1B79A29A1B85E33FED9417233BD3D6A90E6B4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emrenopnftlamb1</t>
   </si>
   <si>
     <t xml:space="preserve">tx hash on that chain</t>
@@ -303,7 +306,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -329,10 +332,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -416,7 +415,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -502,7 +501,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -521,10 +520,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -546,7 +545,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -565,10 +564,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -590,7 +589,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -609,11 +608,11 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>44</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -634,7 +633,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -653,10 +652,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -692,25 +691,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>45</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -746,25 +745,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>45</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -800,25 +799,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>45</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -854,25 +853,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>45</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -908,25 +907,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>45</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -962,25 +961,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>45</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1059,25 +1058,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>45</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1113,25 +1112,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>45</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1168,138 +1167,138 @@
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.44"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.44"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.44"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.44"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.44"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.44"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1321,7 +1320,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1342,7 +1341,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1352,49 +1351,22 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>28</v>
-      </c>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0"/>
+      <c r="B5" s="0"/>
+      <c r="C5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>30</v>
-      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1415,7 +1387,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1436,50 +1408,34 @@
         <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>33</v>
+        <v>24</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>34</v>
-      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0"/>
+      <c r="B4" s="0"/>
+      <c r="C4" s="0"/>
+      <c r="D4" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -1522,21 +1478,21 @@
         <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>38</v>
+        <v>27</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1580,21 +1536,21 @@
         <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1615,8 +1571,8 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1638,21 +1594,21 @@
         <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1673,8 +1629,8 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N23" activeCellId="0" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1693,10 +1649,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1718,7 +1674,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1737,10 +1693,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>